<commit_message>
Update UTwr_Allocation Schema Mapping to WaDE.xlsx
</commit_message>
<xml_diff>
--- a/Utah/WaterAllocation/UTwr_Allocation Schema Mapping to WaDE.xlsx
+++ b/Utah/WaterAllocation/UTwr_Allocation Schema Mapping to WaDE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Utah\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9FF1AE-B762-4A28-9202-397E86BE0E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0461D71D-2EE6-4A8A-BCA8-D9C42BCC1DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="12" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="297">
   <si>
     <t>Name</t>
   </si>
@@ -279,9 +279,6 @@
     <t>OrganizationContactEmail</t>
   </si>
   <si>
-    <t>OrganizationDataMappingURL</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -603,9 +600,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>concantate with a counter and 'UT'</t>
-  </si>
-  <si>
     <t>OwnerClassificationCV</t>
   </si>
   <si>
@@ -702,9 +696,6 @@
     <t>SOURCE</t>
   </si>
   <si>
-    <t>*use keyword search</t>
-  </si>
-  <si>
     <t>OWNER</t>
   </si>
   <si>
@@ -796,12 +787,6 @@
   </si>
   <si>
     <t>"Return" : "Surface Water",</t>
-  </si>
-  <si>
-    <t>"Drain" : "Surface Water",</t>
-  </si>
-  <si>
-    <t>"Spring" : "Surface Water",</t>
   </si>
   <si>
     <t>"Rediversion" : "Surface Water",</t>
@@ -841,15 +826,9 @@
     <t>AllocationUUID</t>
   </si>
   <si>
-    <t>UTwr_WR + counter</t>
-  </si>
-  <si>
     <t>PrimaryBeneficialUseCategory</t>
   </si>
   <si>
-    <t>The Point of Diversion feature class is a complete record of point of diversion locations taken from the Division's day to day operating database. The database is a complete record with the following exceptions:1) The Division's point of diversion referencing policy includes a provision which allows some point of diversion locations to be described more as areas (Point-to-Point Filings) than discrete points. Point to point filings are usually limited to stock watering rights. They are represented  by a discrete point which is located within the area covered by the point to point description.2) Utah State Law required applications to divert surface water to be filed with the State Engineer after 1903 and groundwater after 1935. There may be existing diversions which began prior to those dates which are not included in the Division of Water Right records. The Division becomes aware of these rights and includes these rights in it's records when the user submits a statement of water user claim either pursuant to an adjudication or to establish there is a water right under which the State Engineer is to take action.3) Data in the Division of Water Rights database was entered over an eight year period from paper files maintained by the office. Data entered in the database has been subsequently verified by staff. However, errors are occasionally detected in the database as a result of entry operations either from current staff activities or the original entry project. The Division makes an ongoing effort to maintain the database free of errors and omissions, however users of the data are responsible to verify it is suitable for their purpose. The Division appreciates and encourages users to promptly disclose any inconsistencies detected in the data to Division staff who will make every effort to correct any errors discovered.</t>
-  </si>
-  <si>
     <t>Utah Water Rights Method</t>
   </si>
   <si>
@@ -881,6 +860,82 @@
   </si>
   <si>
     <t>For POU data, the WRNUMS comes in a comma separated list.  We need to explode this data on on WRUNMs before we can work on it, then rename to WRNUM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'UTwr_WS' + native WS id or cutom row counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'UTwr_S' + native S id or cutom row counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'UTwr_WR + native WR id or cutom row counter</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Canal = ["canal", "canals"]</t>
+  </si>
+  <si>
+    <t>Creek =  ["creek"]</t>
+  </si>
+  <si>
+    <t>Ditch = ["ditch"]</t>
+  </si>
+  <si>
+    <t>Drain = ["drain", "drains"]</t>
+  </si>
+  <si>
+    <t>Lake =  ["lake"]</t>
+  </si>
+  <si>
+    <t>Pond = pondList = ["pond"]</t>
+  </si>
+  <si>
+    <t>Reservoir  = ["reservoir"]</t>
+  </si>
+  <si>
+    <t>River = riverList =  ["river", "fork", "surface"]</t>
+  </si>
+  <si>
+    <t>Slough  =  ["slough"]</t>
+  </si>
+  <si>
+    <t>Spring = springList = ["spring", "springs", "gulch", "seep"]</t>
+  </si>
+  <si>
+    <t>Tunnel  =  ["tunnel", "tunnels"]</t>
+  </si>
+  <si>
+    <t>Wash  =  ["wash"]</t>
+  </si>
+  <si>
+    <t>Well = ["well", "wells", "well:", "draw", "hollow"]</t>
+  </si>
+  <si>
+    <t>SiteTypeCV (how was this made / determined?)</t>
+  </si>
+  <si>
+    <t>"Drain" : "Surface and Groundwater",</t>
+  </si>
+  <si>
+    <t>"Spring" : "Groundwater",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Surface and Groundwater</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Surface Water</t>
+  </si>
+  <si>
+    <t>The Point of Diversion feature class is a complete record of point of diversion locations taken from the Division's day to day operating database. The database is a complete record with the following exceptions:1) The Division's point of diversion referencing policy includes a provision which allows some point of diversion locations to be described more as areas (Point-to-Point Filings) than discrete points. Point to point filings are usually limited to stock watering rights. They are represented  by a discrete point which is located within the area covered by the point to point description.2) Utah State Law required applications to divert surface water to be filed with the State Engineer after 1903 and groundwater after 1935. There may be existing diversions which began prior to those dates which are not included in the Division of Water Right records. The Division becomes aware of these rights and includes these rights in it's records when the user submits a statement of water user claim either pursuant to an adjudication or to establish there is a water right under which the State Engineer is to take action.3) Data in the Division of Water Rights database was entered over an eight year period from paper files maintained by the office. Data entered in the database has been subsequently verified by staff. However, errors are occasionally detected in the database as a result of entry operations either from current staff activities or the original entry project. The Division makes an ongoing effort to maintain the database free of errors and omissions, however users of the data are responsible to verify it is suitable for their purpose. The Division appreciates and encourages users to promptly disclose any inconsistencies detected in the data to Division staff who will make every effort to correct any errors discovered.
+What are supplemental numbers and use groups?
+Water right uses (location and type of use) are organized into groups in Division of Water Rights records. Each group is given a unique number by which it is referenced by the water right(s) which share the use. Groups exist to allow the Division to organize records and quantify amounts related to a use. If more than one water right is used to provide water for a use, the water rights which have been grouped together are called supplemental water rights. The idea being that each of the water rights contributes to the beneficial use. Ultimately, quantifying a water right involves determining its sole supply contributed to each use. The group quantifies the extent of the use for the group, while the sole supply defines the contribution of each of the supplemental rights towards the group use. A change or segregation which involves a group necessarily requires that the sole supply of each right in the group be quantified.
+Shared uses (supplemental water rights) may come to light in different ways. Sometimes they are mentioned in applications to appropriate. They may be identified during the approval process, or as the uses of the water are quantified and documented in the proof process. The most common time for supplemental uses to be identified is during the adjudication process as all the water rights and uses in an area are being reviewed and quantified. The important point is that understanding the relationship between uses and the water rights that supply water for the use is critical to determine the water being used and evaluate water rights as new uses are contemplated.
+For more info, visit: https://www.waterrights.utah.gov/wrinfo/faq.asp#q6</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1717,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1912,12 +1967,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1939,14 +1988,14 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="42" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2305,8 +2354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE138B66-616D-4172-8AF0-472ECC34BD33}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2320,54 +2369,54 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="74" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="74" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="74" t="s">
-        <v>192</v>
-      </c>
-      <c r="B6" s="96" t="s">
-        <v>277</v>
+        <v>190</v>
+      </c>
+      <c r="B6" s="93" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>278</v>
+      <c r="B7" s="93" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="74" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="97" t="s">
-        <v>272</v>
+      <c r="B14" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2399,6 +2448,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{C2155799-F85A-42FE-BC14-CFC9E5DF0EBE}"/>
+    <hyperlink ref="B7" r:id="rId2" xr:uid="{A75D0F1C-381E-41A1-82A6-237599122E95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2406,10 +2456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2606DDD-D901-4365-BB8D-3E6142C84460}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2448,13 +2498,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -2512,7 +2562,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="69" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>38</v>
@@ -2524,7 +2574,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>38</v>
@@ -2544,7 +2594,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>38</v>
@@ -2556,7 +2606,7 @@
         <v>38</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>38</v>
@@ -2576,7 +2626,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>38</v>
@@ -2608,7 +2658,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>38</v>
@@ -2640,7 +2690,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>38</v>
@@ -2658,7 +2708,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -2671,8 +2721,8 @@
       <c r="D9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="94" t="s">
-        <v>268</v>
+      <c r="E9" s="95" t="s">
+        <v>296</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>38</v>
@@ -2684,7 +2734,7 @@
         <v>38</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>38</v>
@@ -2704,7 +2754,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>38</v>
@@ -2716,7 +2766,7 @@
         <v>38</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>38</v>
@@ -2735,8 +2785,8 @@
       <c r="D11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="95" t="s">
-        <v>270</v>
+      <c r="E11" s="92" t="s">
+        <v>263</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>38</v>
@@ -2748,7 +2798,7 @@
         <v>38</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>38</v>
@@ -2768,7 +2818,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>38</v>
@@ -2780,9 +2830,38 @@
         <v>38</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J12" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2803,7 +2882,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E4" sqref="E4:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2842,13 +2921,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -2906,7 +2985,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>38</v>
@@ -2918,7 +2997,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>38</v>
@@ -2970,7 +3049,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>38</v>
@@ -2982,7 +3061,7 @@
         <v>38</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>38</v>
@@ -3002,7 +3081,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>38</v>
@@ -3014,7 +3093,7 @@
         <v>38</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>38</v>
@@ -3034,7 +3113,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>38</v>
@@ -3046,7 +3125,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>38</v>
@@ -3066,7 +3145,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>38</v>
@@ -3078,7 +3157,7 @@
         <v>38</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>38</v>
@@ -3130,7 +3209,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>38</v>
@@ -3142,7 +3221,7 @@
         <v>38</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>38</v>
@@ -3162,7 +3241,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>38</v>
@@ -3174,7 +3253,7 @@
         <v>38</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>38</v>
@@ -3194,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>38</v>
@@ -3206,7 +3285,7 @@
         <v>38</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>38</v>
@@ -3223,10 +3302,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8BA2FE-2555-4166-A4DF-0203EE1C77D7}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3265,13 +3344,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -3329,7 +3408,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>38</v>
@@ -3341,7 +3420,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>38</v>
@@ -3361,7 +3440,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F5" s="23" t="s">
         <v>38</v>
@@ -3373,7 +3452,7 @@
         <v>38</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>38</v>
@@ -3393,7 +3472,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>38</v>
@@ -3405,15 +3484,15 @@
         <v>38</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>34</v>
@@ -3424,7 +3503,7 @@
       <c r="D7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="F7" s="23" t="s">
@@ -3437,15 +3516,15 @@
         <v>38</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>34</v>
@@ -3456,7 +3535,7 @@
       <c r="D8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="31" t="s">
         <v>166</v>
       </c>
       <c r="F8" s="23" t="s">
@@ -3469,7 +3548,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>38</v>
@@ -3477,13 +3556,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>38</v>
@@ -3501,21 +3580,21 @@
         <v>38</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>38</v>
@@ -3533,18 +3612,18 @@
         <v>38</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>38</v>
@@ -3552,7 +3631,7 @@
       <c r="D11" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="22" t="s">
         <v>169</v>
       </c>
       <c r="F11" s="23" t="s">
@@ -3565,43 +3644,14 @@
         <v>38</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>38</v>
-      </c>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19"/>
@@ -3624,12 +3674,9 @@
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:A25">
-    <sortCondition ref="A17:A25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:A24">
+    <sortCondition ref="A16:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3641,7 +3688,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3680,13 +3727,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
@@ -3742,7 +3789,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>38</v>
@@ -3754,7 +3801,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="11"/>
     </row>
@@ -3772,7 +3819,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="82" t="s">
         <v>38</v>
@@ -3802,7 +3849,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F6" s="82" t="s">
         <v>38</v>
@@ -3832,7 +3879,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" s="82" t="s">
         <v>38</v>
@@ -3844,7 +3891,7 @@
         <v>38</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J7" s="11"/>
     </row>
@@ -3862,19 +3909,19 @@
         <v>38</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>38</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>214</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>38</v>
+        <v>217</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J8" s="25"/>
     </row>
@@ -3892,7 +3939,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F9" s="82" t="s">
         <v>38</v>
@@ -3922,19 +3969,19 @@
         <v>20</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H10" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J10" s="25"/>
     </row>
@@ -3960,7 +4007,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:G18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3999,13 +4046,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>4</v>
@@ -4061,7 +4108,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>187</v>
+        <v>274</v>
       </c>
       <c r="F4" s="23" t="s">
         <v>38</v>
@@ -4076,12 +4123,12 @@
         <v>38</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B5" s="60" t="s">
         <v>67</v>
@@ -4093,7 +4140,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>38</v>
@@ -4121,22 +4168,22 @@
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="D6" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="92" t="s">
-        <v>259</v>
-      </c>
-      <c r="F6" s="92"/>
-      <c r="G6" s="93"/>
+      <c r="E6" s="90" t="s">
+        <v>254</v>
+      </c>
+      <c r="F6" s="90"/>
+      <c r="G6" s="91"/>
       <c r="H6" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="91" t="s">
-        <v>258</v>
+      <c r="J6" s="89" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -4144,7 +4191,7 @@
         <v>58</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>18</v>
@@ -4153,7 +4200,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F7" s="29" t="s">
         <v>38</v>
@@ -4168,7 +4215,7 @@
         <v>38</v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -4185,7 +4232,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>38</v>
@@ -4200,7 +4247,7 @@
         <v>38</v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -4208,7 +4255,7 @@
         <v>66</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>18</v>
@@ -4217,7 +4264,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>38</v>
@@ -4249,7 +4296,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>38</v>
@@ -4264,7 +4311,7 @@
         <v>38</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -4281,7 +4328,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>38</v>
@@ -4311,7 +4358,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F12" s="29" t="s">
         <v>38</v>
@@ -4334,7 +4381,7 @@
         <v>64</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>18</v>
@@ -4343,7 +4390,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>38</v>
@@ -4366,7 +4413,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>18</v>
@@ -4375,7 +4422,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>38</v>
@@ -4407,10 +4454,10 @@
         <v>38</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G15" s="24" t="s">
         <v>55</v>
@@ -4422,7 +4469,7 @@
         <v>38</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -4439,10 +4486,10 @@
         <v>38</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G16" s="24" t="s">
         <v>54</v>
@@ -4471,7 +4518,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>38</v>
@@ -4503,7 +4550,7 @@
         <v>20</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F18" s="29" t="s">
         <v>38</v>
@@ -4523,7 +4570,7 @@
     </row>
     <row r="19" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>16</v>
@@ -4535,7 +4582,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="80" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F19" s="40" t="s">
         <v>38</v>
@@ -4548,7 +4595,7 @@
       </c>
       <c r="I19" s="81"/>
       <c r="J19" s="83" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -4563,13 +4610,13 @@
         <v>38</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>38</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>219</v>
+        <v>38</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>38</v>
@@ -4578,7 +4625,7 @@
         <v>38</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="24" x14ac:dyDescent="0.3">
@@ -4595,13 +4642,13 @@
         <v>38</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F21" s="29" t="s">
         <v>38</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>38</v>
@@ -4627,7 +4674,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F22" s="29" t="s">
         <v>38</v>
@@ -4642,7 +4689,7 @@
         <v>38</v>
       </c>
       <c r="J22" s="84" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -4658,14 +4705,14 @@
       <c r="D23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="85" t="s">
-        <v>220</v>
-      </c>
-      <c r="F23" s="40" t="s">
-        <v>216</v>
-      </c>
-      <c r="G23" s="86" t="s">
-        <v>219</v>
+      <c r="E23" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="H23" s="11" t="s">
         <v>38</v>
@@ -4674,7 +4721,7 @@
         <v>38</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -4691,7 +4738,7 @@
         <v>20</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>38</v>
@@ -4706,7 +4753,7 @@
         <v>38</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -4723,7 +4770,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F25" s="29" t="s">
         <v>38</v>
@@ -4754,8 +4801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4794,13 +4841,13 @@
         <v>37</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>4</v>
@@ -4814,7 +4861,7 @@
     </row>
     <row r="3" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="60" t="s">
         <v>33</v>
@@ -4968,7 +5015,7 @@
     </row>
     <row r="8" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="59" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B8" s="60" t="s">
         <v>34</v>
@@ -4979,8 +5026,8 @@
       <c r="D8" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>266</v>
+      <c r="E8" s="23" t="s">
+        <v>275</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="56"/>
@@ -5002,7 +5049,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="68" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F9" s="40" t="s">
         <v>38</v>
@@ -5034,7 +5081,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>38</v>
@@ -5066,13 +5113,13 @@
         <v>38</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>38</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H11" s="46" t="s">
         <v>38</v>
@@ -5097,8 +5144,8 @@
       <c r="D12" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="89" t="s">
-        <v>261</v>
+      <c r="E12" s="87" t="s">
+        <v>256</v>
       </c>
       <c r="F12" s="55" t="s">
         <v>38</v>
@@ -5118,7 +5165,7 @@
     </row>
     <row r="13" spans="1:10" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B13" s="60" t="s">
         <v>33</v>
@@ -5130,7 +5177,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F13" s="40" t="s">
         <v>38</v>
@@ -5150,7 +5197,7 @@
     </row>
     <row r="14" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>68</v>
@@ -5162,7 +5209,7 @@
         <v>38</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F14" s="40" t="s">
         <v>38</v>
@@ -5177,12 +5224,12 @@
         <v>38</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>68</v>
@@ -5194,7 +5241,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F15" s="40" t="s">
         <v>38</v>
@@ -5209,12 +5256,12 @@
         <v>38</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="60" t="s">
         <v>34</v>
@@ -5226,7 +5273,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F16" s="40" t="s">
         <v>38</v>
@@ -5241,12 +5288,12 @@
         <v>38</v>
       </c>
       <c r="J16" s="64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>15</v>
@@ -5258,7 +5305,7 @@
         <v>38</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" s="40" t="s">
         <v>38</v>
@@ -5273,12 +5320,12 @@
         <v>38</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>34</v>
@@ -5290,13 +5337,13 @@
         <v>38</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F18" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H18" s="46" t="s">
         <v>38</v>
@@ -5305,12 +5352,12 @@
         <v>38</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>69</v>
@@ -5322,7 +5369,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F19" s="40" t="s">
         <v>38</v>
@@ -5342,7 +5389,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>33</v>
@@ -5354,7 +5401,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F20" s="40" t="s">
         <v>38</v>
@@ -5374,7 +5421,7 @@
     </row>
     <row r="21" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>69</v>
@@ -5389,10 +5436,10 @@
         <v>38</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" s="46" t="s">
         <v>38</v>
@@ -5406,7 +5453,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>34</v>
@@ -5418,13 +5465,13 @@
         <v>20</v>
       </c>
       <c r="E22" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H22" s="46" t="s">
         <v>38</v>
@@ -5433,12 +5480,12 @@
         <v>38</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>34</v>
@@ -5453,10 +5500,10 @@
         <v>38</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H23" s="46" t="s">
         <v>38</v>
@@ -5465,7 +5512,7 @@
         <v>38</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -5476,7 +5523,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>34</v>
@@ -5491,10 +5538,10 @@
         <v>38</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H24" s="46" t="s">
         <v>38</v>
@@ -5503,12 +5550,12 @@
         <v>38</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>33</v>
@@ -5523,10 +5570,10 @@
         <v>38</v>
       </c>
       <c r="F25" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>38</v>
@@ -5535,12 +5582,12 @@
         <v>38</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>15</v>
@@ -5552,7 +5599,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F26" s="40" t="s">
         <v>38</v>
@@ -5572,10 +5619,10 @@
     </row>
     <row r="27" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>18</v>
@@ -5584,7 +5631,7 @@
         <v>38</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F27" s="40" t="s">
         <v>38</v>
@@ -5604,10 +5651,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>18</v>
@@ -5616,7 +5663,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F28" s="40" t="s">
         <v>38</v>
@@ -5636,7 +5683,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>34</v>
@@ -5648,7 +5695,7 @@
         <v>20</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F29" s="29" t="s">
         <v>38</v>
@@ -5663,12 +5710,12 @@
         <v>38</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>69</v>
@@ -5680,7 +5727,7 @@
         <v>38</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F30" s="40" t="s">
         <v>38</v>
@@ -5706,7 +5753,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>34</v>
@@ -5718,13 +5765,13 @@
         <v>38</v>
       </c>
       <c r="E31" s="73" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F31" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H31" s="46" t="s">
         <v>38</v>
@@ -5738,7 +5785,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>34</v>
@@ -5750,7 +5797,7 @@
         <v>38</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F32" s="40" t="s">
         <v>38</v>
@@ -5765,12 +5812,12 @@
         <v>38</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>15</v>
@@ -5782,7 +5829,7 @@
         <v>20</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F33" s="40" t="s">
         <v>38</v>
@@ -5797,12 +5844,12 @@
         <v>38</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>15</v>
@@ -5814,7 +5861,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F34" s="40" t="s">
         <v>38</v>
@@ -5829,7 +5876,7 @@
         <v>38</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
@@ -5840,7 +5887,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B35" s="60" t="s">
         <v>33</v>
@@ -5852,7 +5899,7 @@
         <v>38</v>
       </c>
       <c r="E35" s="72" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F35" s="40" t="s">
         <v>38</v>
@@ -5878,7 +5925,7 @@
     </row>
     <row r="36" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>15</v>
@@ -5890,7 +5937,7 @@
         <v>38</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F36" s="40" t="s">
         <v>38</v>
@@ -5916,10 +5963,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="77" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B37" s="60" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C37" s="61" t="s">
         <v>18</v>
@@ -5950,7 +5997,7 @@
     </row>
     <row r="38" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="60" t="s">
         <v>69</v>
@@ -5962,12 +6009,12 @@
         <v>38</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F38" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="87" t="s">
+      <c r="G38" s="85" t="s">
         <v>38</v>
       </c>
       <c r="H38" s="65" t="s">
@@ -5982,7 +6029,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>69</v>
@@ -5997,10 +6044,10 @@
         <v>38</v>
       </c>
       <c r="F39" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H39" s="46" t="s">
         <v>38</v>
@@ -6014,7 +6061,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>15</v>
@@ -6026,7 +6073,7 @@
         <v>20</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F40" s="40" t="s">
         <v>38</v>
@@ -6041,12 +6088,12 @@
         <v>38</v>
       </c>
       <c r="J40" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>34</v>
@@ -6058,7 +6105,7 @@
         <v>38</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F41" s="40" t="s">
         <v>38</v>
@@ -6084,7 +6131,7 @@
     </row>
     <row r="42" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="59" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B42" s="60" t="s">
         <v>34</v>
@@ -6096,12 +6143,12 @@
         <v>20</v>
       </c>
       <c r="E42" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F42" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G42" s="87" t="s">
+      <c r="G42" s="85" t="s">
         <v>38</v>
       </c>
       <c r="H42" s="65" t="s">
@@ -6110,13 +6157,13 @@
       <c r="I42" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="J42" s="88" t="s">
-        <v>189</v>
+      <c r="J42" s="86" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>33</v>
@@ -6128,7 +6175,7 @@
         <v>38</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F43" s="40" t="s">
         <v>38</v>
@@ -6148,7 +6195,7 @@
     </row>
     <row r="44" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>16</v>
@@ -6160,7 +6207,7 @@
         <v>20</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F44" s="40" t="s">
         <v>38</v>
@@ -6175,7 +6222,7 @@
         <v>38</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
@@ -6186,10 +6233,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="59" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B45" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="61" t="s">
         <v>18</v>
@@ -6198,7 +6245,7 @@
         <v>20</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" s="29" t="s">
         <v>38</v>
@@ -6213,7 +6260,7 @@
         <v>38</v>
       </c>
       <c r="J45" s="64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K45" s="59"/>
       <c r="L45" s="59"/>
@@ -6224,7 +6271,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>34</v>
@@ -6236,7 +6283,7 @@
         <v>38</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F46" s="40" t="s">
         <v>38</v>
@@ -6251,7 +6298,7 @@
         <v>38</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -6266,298 +6313,375 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A68CD9-E6C8-4C1E-8A36-F76F66BA5935}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="71" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="B3" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="71" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="B4" s="71" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="71" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="71" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="71" t="s">
+      <c r="B5" s="71" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="71" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="71" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="71" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="71" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="71" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="71" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="B7" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="71" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="71" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="71" t="s">
+      <c r="B8" s="71" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="71" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="94" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="94" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C16" s="94" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C17" s="94" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C18" s="94" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C19" s="94" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C20" s="94" t="s">
+        <v>285</v>
+      </c>
+      <c r="L20" s="94"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C21" s="94" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C22" s="94" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C23" s="94" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C24" s="94" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="F29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+      <c r="F30" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+      <c r="F32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="F33" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>252</v>
-      </c>
-      <c r="J35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="F34" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>242</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:A34">
+    <sortCondition ref="A27:A34"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>